<commit_message>
deleted old copy of notebook, also updated a spreadsheet
</commit_message>
<xml_diff>
--- a/part-1-experiment.xlsx
+++ b/part-1-experiment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brent\Documents\code\course22\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E005C031-57F5-40D6-B1C0-D0C5930AC70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D47F703-6EB3-486C-A97C-DA4019174B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10485" yWindow="390" windowWidth="18795" windowHeight="20835" xr2:uid="{C994DD87-F745-4EA9-9D8C-3FBDAE41A79E}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,354 +424,362 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(0,5)</f>
+        <v>3</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B38" si="0">A3*2</f>
-        <v>10</v>
+        <f t="shared" ref="B3:B38" ca="1" si="0">A3*2</f>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <f t="shared" ref="A4:A38" ca="1" si="1">RANDBETWEEN(0,5)</f>
+        <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>19</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>35</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>70</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>57</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>114</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>86</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>172</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>87</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>174</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>103</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>206</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>46</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" ref="A12:A38" ca="1" si="1">RANDBETWEEN(0,100)</f>
-        <v>75</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>150</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>156</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>172</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>168</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>196</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>90</v>
+        <v>2</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>180</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" ca="1" si="1"/>
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>114</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" ca="1" si="1"/>
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>164</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>44</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>48</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" ca="1" si="1"/>
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>176</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" ca="1" si="1"/>
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>188</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>